<commit_message>
Add the business transaction of 25/04/2018
</commit_message>
<xml_diff>
--- a/项目计划与进度/改2018年基层信息化实施推进情况表.xlsx
+++ b/项目计划与进度/改2018年基层信息化实施推进情况表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22943" windowHeight="9947" activeTab="1"/>
+    <workbookView windowWidth="22943" windowHeight="9540"/>
   </bookViews>
   <sheets>
     <sheet name="委属" sheetId="3" r:id="rId1"/>
@@ -137,6 +137,9 @@
     <t>发行量</t>
   </si>
   <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
     <t>受理量</t>
   </si>
   <si>
@@ -357,9 +360,6 @@
   </si>
   <si>
     <t>区卫计委</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>设备准备</t>
@@ -456,18 +456,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="30">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -542,8 +535,39 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -558,7 +582,76 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -579,114 +672,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="37">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -719,43 +712,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -767,25 +730,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -803,13 +754,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -821,7 +820,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -833,7 +832,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -845,61 +880,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1011,6 +998,45 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1031,36 +1057,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1094,15 +1090,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -1116,10 +1103,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="32" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1128,19 +1115,19 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1149,112 +1136,112 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1307,7 +1294,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1322,106 +1309,106 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1772,14 +1759,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:U28"/>
+  <dimension ref="A1:W28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E19" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="U14" sqref="U14"/>
+      <selection pane="bottomRight" activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="10.8"/>
@@ -1953,7 +1940,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" ht="20.1" customHeight="1" spans="1:21">
+    <row r="4" ht="20.1" customHeight="1" spans="1:23">
       <c r="A4" s="33"/>
       <c r="B4" s="34"/>
       <c r="C4" s="35"/>
@@ -2009,13 +1996,20 @@
       <c r="U4" s="34">
         <v>545</v>
       </c>
-    </row>
-    <row r="5" ht="20.1" customHeight="1" spans="1:21">
+      <c r="V4" s="27">
+        <f>SUM(E4:U4)</f>
+        <v>214704</v>
+      </c>
+      <c r="W4" s="27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" ht="20.1" customHeight="1" spans="1:22">
       <c r="A5" s="33"/>
       <c r="B5" s="34"/>
       <c r="C5" s="35"/>
       <c r="D5" s="36" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E5" s="34">
         <v>1274</v>
@@ -2065,6 +2059,10 @@
       </c>
       <c r="U5" s="34">
         <v>1098</v>
+      </c>
+      <c r="V5" s="27">
+        <f>SUM(E5:U5)</f>
+        <v>25331</v>
       </c>
     </row>
     <row r="6" ht="24" spans="1:21">
@@ -2072,113 +2070,113 @@
       <c r="B6" s="34"/>
       <c r="C6" s="37"/>
       <c r="D6" s="36" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E6" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F6" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G6" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H6" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I6" s="38"/>
       <c r="J6" s="38" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K6" s="38" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L6" s="38" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M6" s="38"/>
       <c r="N6" s="38" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="O6" s="38" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="P6" s="38" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="Q6" s="38" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="R6" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="S6" s="38"/>
       <c r="T6" s="38" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="U6" s="38" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" ht="27" customHeight="1" spans="1:21">
       <c r="A7" s="33"/>
       <c r="B7" s="34"/>
       <c r="C7" s="39" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E7" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F7" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G7" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H7" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I7" s="38" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J7" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K7" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L7" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M7" s="38" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N7" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="O7" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="P7" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Q7" s="38" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="R7" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="S7" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="T7" s="38" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="U7" s="38" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" ht="24" customHeight="1" spans="1:21">
@@ -2186,7 +2184,7 @@
       <c r="B8" s="34"/>
       <c r="C8" s="35"/>
       <c r="D8" s="36" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E8" s="38">
         <v>99.67</v>
@@ -2237,113 +2235,113 @@
       <c r="B9" s="34"/>
       <c r="C9" s="37"/>
       <c r="D9" s="36" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E9" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F9" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G9" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H9" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I9" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J9" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K9" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L9" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M9" s="38" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="N9" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="O9" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="P9" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Q9" s="38" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="R9" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="S9" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="T9" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="U9" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" ht="27" customHeight="1" spans="1:21">
       <c r="A10" s="33"/>
       <c r="B10" s="39" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C10" s="35" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D10" s="36" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E10" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F10" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G10" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H10" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I10" s="38"/>
       <c r="J10" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K10" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L10" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M10" s="38"/>
       <c r="N10" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="O10" s="38" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="P10" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Q10" s="38"/>
       <c r="R10" s="38"/>
       <c r="S10" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="T10" s="38" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="U10" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" ht="24" customHeight="1" spans="1:21">
@@ -2351,105 +2349,105 @@
       <c r="B11" s="35"/>
       <c r="C11" s="35"/>
       <c r="D11" s="36" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E11" s="40" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F11" s="38" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G11" s="38"/>
       <c r="H11" s="38" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I11" s="38"/>
       <c r="J11" s="38" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="K11" s="38" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L11" s="38" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="M11" s="38"/>
       <c r="N11" s="38" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="O11" s="38" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="P11" s="38" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q11" s="38" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="R11" s="38" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="S11" s="38" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="T11" s="38" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="U11" s="38" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" ht="27.95" customHeight="1" spans="1:21">
       <c r="A12" s="33"/>
       <c r="B12" s="35"/>
       <c r="C12" s="39" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D12" s="36" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E12" s="40" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F12" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="G12" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="G12" s="38" t="s">
-        <v>66</v>
-      </c>
       <c r="H12" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I12" s="38"/>
       <c r="J12" s="38" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K12" s="38" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L12" s="38" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M12" s="38"/>
       <c r="N12" s="38" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O12" s="38" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="P12" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Q12" s="38"/>
       <c r="R12" s="38"/>
       <c r="S12" s="38" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="T12" s="38" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="U12" s="38" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" ht="24" spans="1:21">
@@ -2457,101 +2455,101 @@
       <c r="B13" s="35"/>
       <c r="C13" s="37"/>
       <c r="D13" s="36" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E13" s="40" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F13" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="G13" s="38" t="s">
-        <v>66</v>
-      </c>
       <c r="H13" s="38" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I13" s="38"/>
       <c r="J13" s="38" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K13" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L13" s="38" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M13" s="38"/>
       <c r="N13" s="38" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O13" s="38" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="P13" s="38" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="Q13" s="38"/>
       <c r="R13" s="38"/>
       <c r="S13" s="38"/>
       <c r="T13" s="38"/>
       <c r="U13" s="38" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" ht="15.95" customHeight="1" spans="1:21">
       <c r="A14" s="33"/>
       <c r="B14" s="35"/>
       <c r="C14" s="35" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D14" s="36" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E14" s="34" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F14" s="34" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G14" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H14" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I14" s="38" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J14" s="38" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K14" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L14" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M14" s="38"/>
       <c r="N14" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="O14" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="P14" s="34" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Q14" s="38"/>
       <c r="R14" s="38" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="S14" s="38"/>
       <c r="T14" s="38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="U14" s="34" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" ht="27.95" customHeight="1" spans="1:21">
@@ -2559,7 +2557,7 @@
       <c r="B15" s="35"/>
       <c r="C15" s="35"/>
       <c r="D15" s="36" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E15" s="34">
         <v>22</v>
@@ -2604,48 +2602,48 @@
       <c r="B16" s="35"/>
       <c r="C16" s="35"/>
       <c r="D16" s="36" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E16" s="40" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F16" s="34" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G16" s="38" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H16" s="38" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I16" s="38"/>
       <c r="J16" s="38" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K16" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L16" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M16" s="38"/>
       <c r="N16" s="38" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="O16" s="41" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="P16" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Q16" s="38"/>
       <c r="R16" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="S16" s="38"/>
       <c r="T16" s="38"/>
       <c r="U16" s="38" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" ht="24" customHeight="1" spans="1:21">
@@ -2653,48 +2651,48 @@
       <c r="B17" s="35"/>
       <c r="C17" s="35"/>
       <c r="D17" s="36" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E17" s="40" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F17" s="38" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G17" s="38" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H17" s="38" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I17" s="38"/>
       <c r="J17" s="38" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K17" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L17" s="38" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M17" s="38"/>
       <c r="N17" s="38" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="O17" s="41" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="P17" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Q17" s="38"/>
       <c r="R17" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="S17" s="38"/>
       <c r="T17" s="38"/>
       <c r="U17" s="38" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" ht="21" customHeight="1" spans="1:21">
@@ -2702,34 +2700,34 @@
       <c r="B18" s="35"/>
       <c r="C18" s="35"/>
       <c r="D18" s="36" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E18" s="34" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F18" s="34" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G18" s="38" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H18" s="38" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I18" s="38"/>
       <c r="J18" s="38" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K18" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L18" s="38"/>
       <c r="M18" s="38"/>
       <c r="N18" s="38" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="O18" s="41" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="P18" s="38"/>
       <c r="Q18" s="38"/>
@@ -2737,7 +2735,7 @@
       <c r="S18" s="38"/>
       <c r="T18" s="38"/>
       <c r="U18" s="38" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" ht="24" customHeight="1" spans="1:21">
@@ -2745,34 +2743,34 @@
       <c r="B19" s="35"/>
       <c r="C19" s="35"/>
       <c r="D19" s="36" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E19" s="40" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F19" s="38" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G19" s="38" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H19" s="38" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I19" s="38"/>
       <c r="J19" s="38" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K19" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L19" s="38"/>
       <c r="M19" s="38"/>
       <c r="N19" s="38" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="O19" s="41" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="P19" s="38"/>
       <c r="Q19" s="38"/>
@@ -2780,7 +2778,7 @@
       <c r="S19" s="38"/>
       <c r="T19" s="38"/>
       <c r="U19" s="38" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" ht="24.95" customHeight="1" spans="1:21">
@@ -2788,109 +2786,109 @@
       <c r="B20" s="35"/>
       <c r="C20" s="35"/>
       <c r="D20" s="36" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E20" s="40" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F20" s="38" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G20" s="38" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H20" s="38" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I20" s="38"/>
       <c r="J20" s="38" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K20" s="38" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L20" s="38" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M20" s="38"/>
       <c r="N20" s="38" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="O20" s="41" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="P20" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Q20" s="38"/>
       <c r="R20" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="S20" s="38"/>
       <c r="T20" s="38"/>
       <c r="U20" s="38" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" ht="24" customHeight="1" spans="1:21">
       <c r="A21" s="33" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B21" s="39" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C21" s="39" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D21" s="42" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E21" s="40" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F21" s="34" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G21" s="34" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H21" s="34" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I21" s="34" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J21" s="38" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K21" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L21" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M21" s="38"/>
       <c r="N21" s="38" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="O21" s="41" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="P21" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Q21" s="38"/>
       <c r="R21" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="S21" s="38" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="T21" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="U21" s="38" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" ht="24" customHeight="1" spans="1:21">
@@ -2898,7 +2896,7 @@
       <c r="B22" s="37"/>
       <c r="C22" s="37"/>
       <c r="D22" s="42" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E22" s="40"/>
       <c r="F22" s="34"/>
@@ -2921,60 +2919,60 @@
     <row r="23" ht="24" spans="1:21">
       <c r="A23" s="33"/>
       <c r="B23" s="42" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C23" s="42" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D23" s="42" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E23" s="40" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F23" s="34" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G23" s="34" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H23" s="34" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I23" s="34" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J23" s="38" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K23" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L23" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M23" s="38"/>
       <c r="N23" s="38" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="O23" s="41" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="P23" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Q23" s="38"/>
       <c r="R23" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="S23" s="38" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="T23" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="U23" s="38" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" s="23" customFormat="1" spans="1:21">
@@ -3002,7 +3000,7 @@
     </row>
     <row r="25" s="24" customFormat="1" ht="15.95" customHeight="1" spans="1:21">
       <c r="A25" s="46" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B25" s="46"/>
       <c r="C25" s="46"/>
@@ -3064,58 +3062,58 @@
       <c r="B26" s="46"/>
       <c r="C26" s="46"/>
       <c r="D26" s="46" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E26" s="49" t="s">
+        <v>88</v>
+      </c>
+      <c r="F26" s="49" t="s">
+        <v>94</v>
+      </c>
+      <c r="G26" s="49" t="s">
+        <v>88</v>
+      </c>
+      <c r="H26" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="F26" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="G26" s="49" t="s">
+      <c r="I26" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="J26" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="K26" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="L26" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="M26" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="N26" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="H26" s="49" t="s">
-        <v>86</v>
-      </c>
-      <c r="I26" s="49" t="s">
-        <v>94</v>
-      </c>
-      <c r="J26" s="49" t="s">
+      <c r="O26" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="P26" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q26" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="R26" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="K26" s="49" t="s">
-        <v>96</v>
-      </c>
-      <c r="L26" s="49" t="s">
-        <v>97</v>
-      </c>
-      <c r="M26" s="49" t="s">
-        <v>95</v>
-      </c>
-      <c r="N26" s="49" t="s">
-        <v>86</v>
-      </c>
-      <c r="O26" s="49" t="s">
-        <v>98</v>
-      </c>
-      <c r="P26" s="49" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q26" s="49" t="s">
-        <v>95</v>
-      </c>
-      <c r="R26" s="49" t="s">
-        <v>94</v>
-      </c>
       <c r="S26" s="49" t="s">
+        <v>88</v>
+      </c>
+      <c r="T26" s="49" t="s">
+        <v>88</v>
+      </c>
+      <c r="U26" s="49" t="s">
         <v>87</v>
-      </c>
-      <c r="T26" s="49" t="s">
-        <v>87</v>
-      </c>
-      <c r="U26" s="49" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="27" s="24" customFormat="1" ht="14.1" customHeight="1" spans="1:21">
@@ -3123,29 +3121,29 @@
       <c r="B27" s="46"/>
       <c r="C27" s="46"/>
       <c r="D27" s="46" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E27" s="46" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F27" s="47" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G27" s="47" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H27" s="46" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I27" s="47"/>
       <c r="J27" s="47" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="K27" s="46" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L27" s="46" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="M27" s="47"/>
       <c r="N27" s="47"/>
@@ -3155,7 +3153,7 @@
       <c r="R27" s="47"/>
       <c r="S27" s="47"/>
       <c r="T27" s="46" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="U27" s="47"/>
     </row>
@@ -3164,25 +3162,25 @@
       <c r="B28" s="46"/>
       <c r="C28" s="46"/>
       <c r="D28" s="46" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E28" s="50" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F28" s="47"/>
       <c r="G28" s="47"/>
       <c r="H28" s="50" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I28" s="50" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J28" s="47"/>
       <c r="K28" s="47"/>
       <c r="L28" s="47"/>
       <c r="M28" s="47"/>
       <c r="N28" s="50" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="O28" s="47"/>
       <c r="P28" s="47"/>
@@ -3221,10 +3219,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.87962962962963" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -3238,50 +3236,50 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" spans="1:6">
       <c r="A2" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="28.8" spans="1:6">
       <c r="A3" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>114</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" ht="28.8" spans="1:6">
@@ -3294,7 +3292,7 @@
         <v>116</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F4" s="6"/>
     </row>
@@ -3308,7 +3306,7 @@
         <v>118</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F5" s="6"/>
     </row>
@@ -3326,7 +3324,7 @@
         <v>122</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F6" s="13"/>
     </row>
@@ -3337,10 +3335,10 @@
         <v>123</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F7" s="13"/>
     </row>
@@ -3352,7 +3350,7 @@
         <v>124</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F8" s="13"/>
     </row>
@@ -3388,7 +3386,7 @@
         <v>128</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F11" s="13"/>
     </row>
@@ -3445,16 +3443,16 @@
     <row r="16" ht="14.1" customHeight="1" spans="1:6">
       <c r="A16" s="9"/>
       <c r="B16" s="14" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>138</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F16" s="13"/>
     </row>
@@ -3474,7 +3472,7 @@
       <c r="A18" s="18"/>
       <c r="B18" s="15"/>
       <c r="C18" s="13" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="13" t="s">
@@ -3482,7 +3480,7 @@
       </c>
       <c r="F18" s="13"/>
     </row>
-    <row r="19" ht="43.2" spans="1:6">
+    <row r="19" spans="1:6">
       <c r="A19" s="12" t="s">
         <v>141</v>
       </c>
@@ -3490,13 +3488,15 @@
         <v>142</v>
       </c>
       <c r="C19" s="20"/>
-      <c r="D19" s="12" t="s">
+      <c r="E19" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="F19" s="13"/>
+    </row>
+    <row r="20" ht="43.2" spans="4:4">
+      <c r="D20" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="E19" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="F19" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>